<commit_message>
Job Title add delete
</commit_message>
<xml_diff>
--- a/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
+++ b/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddJobTitles" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>JobTitle</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>OPENING FOR TESTING</t>
+  </si>
+  <si>
+    <t>ALFA</t>
   </si>
 </sst>
 </file>
@@ -397,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -441,7 +444,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -460,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -480,10 +483,13 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Emp status and Job Category Menus
</commit_message>
<xml_diff>
--- a/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
+++ b/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
@@ -4,20 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AddJobTitles" sheetId="1" r:id="rId1"/>
     <sheet name="DeleteJobTitles" sheetId="2" r:id="rId2"/>
     <sheet name="AddpayGrades" sheetId="3" r:id="rId3"/>
     <sheet name="DeletePayGrade" sheetId="4" r:id="rId4"/>
+    <sheet name="AddEmpStatus" sheetId="5" r:id="rId5"/>
+    <sheet name="DeleteEmpStatus" sheetId="6" r:id="rId6"/>
+    <sheet name="AddJobCategories" sheetId="7" r:id="rId7"/>
+    <sheet name="DeleteJobCategories" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>JobTitle</t>
   </si>
@@ -52,10 +56,31 @@
     <t>PayGrade</t>
   </si>
   <si>
-    <t>LEVEL 3</t>
-  </si>
-  <si>
     <t>LEVEL 5</t>
+  </si>
+  <si>
+    <t>LEVEL 6</t>
+  </si>
+  <si>
+    <t>LEVEL6</t>
+  </si>
+  <si>
+    <t>empStatus</t>
+  </si>
+  <si>
+    <t>TEST1</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>jobCategory</t>
+  </si>
+  <si>
+    <t>TEST1 Jobs</t>
+  </si>
+  <si>
+    <t>TEST2 Jobs</t>
   </si>
 </sst>
 </file>
@@ -453,7 +478,9 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -462,9 +489,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -482,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -524,10 +549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -543,7 +568,12 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -555,7 +585,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,4 +620,159 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
General Info Page Working
</commit_message>
<xml_diff>
--- a/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
+++ b/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AddJobTitles" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="DeleteEmpStatus" sheetId="6" r:id="rId6"/>
     <sheet name="AddJobCategories" sheetId="7" r:id="rId7"/>
     <sheet name="DeleteJobCategories" sheetId="8" r:id="rId8"/>
+    <sheet name="generalInfo" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>JobTitle</t>
   </si>
@@ -81,12 +82,81 @@
   </si>
   <si>
     <t>TEST2 Jobs</t>
+  </si>
+  <si>
+    <t>OrgName</t>
+  </si>
+  <si>
+    <t>TaxId</t>
+  </si>
+  <si>
+    <t>RegNo</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>admin@rohithsingirikonda.tk</t>
+  </si>
+  <si>
+    <t>HYDERABAD</t>
+  </si>
+  <si>
+    <t>GACHIBOWLI</t>
+  </si>
+  <si>
+    <t>TLANGANA</t>
+  </si>
+  <si>
+    <t>ta266te4455</t>
+  </si>
+  <si>
+    <t>This company is related to HR Management System</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -103,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,10 +220,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,4 +853,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1234515588</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4">
+        <v>8888888888</v>
+      </c>
+      <c r="E2" s="4">
+        <v>6666666666</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="4">
+        <v>560032</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4">
+        <v>1234515588</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8888888888</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6666666666</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="4">
+        <v>560032</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LocPage & Add LocationPage Partially completed
</commit_message>
<xml_diff>
--- a/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
+++ b/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="AddJobTitles" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,15 @@
     <sheet name="AddJobCategories" sheetId="7" r:id="rId7"/>
     <sheet name="DeleteJobCategories" sheetId="8" r:id="rId8"/>
     <sheet name="generalInfo" sheetId="9" r:id="rId9"/>
+    <sheet name="DeleteLocations" sheetId="10" r:id="rId10"/>
+    <sheet name="AddLocation" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>JobTitle</t>
   </si>
@@ -148,6 +150,51 @@
   </si>
   <si>
     <t>OrangeHRM</t>
+  </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>BENGALURU</t>
+  </si>
+  <si>
+    <t>CHENNAI</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Los Angles</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>MUMBAI</t>
+  </si>
+  <si>
+    <t>TAMILNADU</t>
+  </si>
+  <si>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Test Company</t>
+  </si>
+  <si>
+    <t>Locations</t>
   </si>
 </sst>
 </file>
@@ -193,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -216,16 +263,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,6 +657,170 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2">
+        <v>570985</v>
+      </c>
+      <c r="G2" s="2">
+        <v>999999999</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
@@ -817,7 +1057,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -859,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Education Validation Add Error Pending
</commit_message>
<xml_diff>
--- a/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
+++ b/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="AddJobTitles" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,16 @@
     <sheet name="AddSkills" sheetId="12" r:id="rId12"/>
     <sheet name="DeleteSkills" sheetId="13" r:id="rId13"/>
     <sheet name="EditSkills" sheetId="14" r:id="rId14"/>
+    <sheet name="AddEducation" sheetId="15" r:id="rId15"/>
+    <sheet name="DeleteEducation" sheetId="16" r:id="rId16"/>
+    <sheet name="EditEducation" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>JobTitle</t>
   </si>
@@ -228,6 +231,24 @@
   </si>
   <si>
     <t>C#</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>SSC</t>
+  </si>
+  <si>
+    <t>BSC</t>
+  </si>
+  <si>
+    <t>existing_Education</t>
+  </si>
+  <si>
+    <t>updated_Education</t>
+  </si>
+  <si>
+    <t>SSC/10TH</t>
   </si>
 </sst>
 </file>
@@ -861,7 +882,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -907,10 +928,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -924,10 +945,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="9"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="9" t="s">
+      <c r="A2" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -940,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -976,6 +994,119 @@
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
         <v>61</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="B4" s="9"/>
     </row>

</xml_diff>

<commit_message>
Language Page Completed and Memberships Partially
</commit_message>
<xml_diff>
--- a/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
+++ b/src/main/java/com/HRM/testdata/Admin_Datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="5145" firstSheet="20" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="AddJobTitles" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,19 @@
     <sheet name="AddLicense" sheetId="18" r:id="rId18"/>
     <sheet name="DeleteLicense" sheetId="19" r:id="rId19"/>
     <sheet name="EditLicense" sheetId="20" r:id="rId20"/>
+    <sheet name="AddLanguage" sheetId="21" r:id="rId21"/>
+    <sheet name="DeleteLanguage" sheetId="24" r:id="rId22"/>
+    <sheet name="EditLanguage" sheetId="23" r:id="rId23"/>
+    <sheet name="AddMembership" sheetId="25" r:id="rId24"/>
+    <sheet name="DeleteMembership" sheetId="26" r:id="rId25"/>
+    <sheet name="EditMembership" sheetId="27" r:id="rId26"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="96">
   <si>
     <t>JobTitle</t>
   </si>
@@ -273,6 +279,54 @@
   </si>
   <si>
     <t>TESTB UPDATED LICENSE</t>
+  </si>
+  <si>
+    <t>KANNADA</t>
+  </si>
+  <si>
+    <t>KANNADIAN</t>
+  </si>
+  <si>
+    <t>existing_Language</t>
+  </si>
+  <si>
+    <t>updated_Language</t>
+  </si>
+  <si>
+    <t>TAMIL</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>Membership</t>
+  </si>
+  <si>
+    <t>ISO CERTIFIED</t>
+  </si>
+  <si>
+    <t>CSI</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>CMML4</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>existing_Membership</t>
+  </si>
+  <si>
+    <t>updated_Membership</t>
+  </si>
+  <si>
+    <t>CSI_NEW</t>
   </si>
 </sst>
 </file>
@@ -369,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -382,6 +436,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1144,7 +1201,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1180,7 +1237,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1248,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1284,6 +1341,256 @@
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
         <v>75</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="B4" s="9"/>
     </row>

</xml_diff>